<commit_message>
Revert "Resolve issue #60."
</commit_message>
<xml_diff>
--- a/test/summary/summary_test02_out.xlsx
+++ b/test/summary/summary_test02_out.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>11/18/16</t>
-  </si>
-  <si>
-    <t>11/21/16</t>
   </si>
 </sst>
 </file>
@@ -199,23 +196,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="0">
-        <v>0</v>
-      </c>
-      <c r="C4" s="0">
-        <v>20</v>
-      </c>
-      <c r="D4" s="0">
-        <v>0</v>
-      </c>
-      <c r="E4" s="0">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixes issue 23, updating ado and test files
</commit_message>
<xml_diff>
--- a/test/summary/summary_test02_out.xlsx
+++ b/test/summary/summary_test02_out.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>11/21/16</t>
+  </si>
+  <si>
+    <t>12/20/16</t>
   </si>
 </sst>
 </file>
@@ -113,6 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P5"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -216,6 +220,23 @@
         <v>20</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="0">
+        <v>0</v>
+      </c>
+      <c r="C5" s="0">
+        <v>20</v>
+      </c>
+      <c r="D5" s="0">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>